<commit_message>
before testing different binning parameters
</commit_message>
<xml_diff>
--- a/hw2/scorecards/scorecards.xlsx
+++ b/hw2/scorecards/scorecards.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E116"/>
+  <dimension ref="A1:E112"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,7 +475,7 @@
         <v>-0.1053605156567152</v>
       </c>
       <c r="D2" t="n">
-        <v>0.6066014888502654</v>
+        <v>0.6801689867974033</v>
       </c>
       <c r="E2" t="n">
         <v>8</v>
@@ -496,10 +496,10 @@
         <v>0.09531017979323402</v>
       </c>
       <c r="D3" t="n">
-        <v>0.6066014888502654</v>
+        <v>0.6801689867974033</v>
       </c>
       <c r="E3" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
@@ -517,10 +517,10 @@
         <v>-0.5951667721187759</v>
       </c>
       <c r="D4" t="n">
-        <v>0.6066014888502654</v>
+        <v>0.6801689867974033</v>
       </c>
       <c r="E4" t="n">
-        <v>-1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="5">
@@ -538,7 +538,7 @@
         <v>-0.04457963162867034</v>
       </c>
       <c r="D5" t="n">
-        <v>0.6066014888502654</v>
+        <v>0.6801689867974033</v>
       </c>
       <c r="E5" t="n">
         <v>9</v>
@@ -559,10 +559,10 @@
         <v>0.2430621945988553</v>
       </c>
       <c r="D6" t="n">
-        <v>0.6066014888502654</v>
+        <v>0.6801689867974033</v>
       </c>
       <c r="E6" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7">
@@ -580,10 +580,10 @@
         <v>0.493086799388584</v>
       </c>
       <c r="D7" t="n">
-        <v>0.6066014888502654</v>
+        <v>0.6801689867974033</v>
       </c>
       <c r="E7" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8">
@@ -601,10 +601,10 @@
         <v>-0.07410797214960101</v>
       </c>
       <c r="D8" t="n">
-        <v>0.6066014888502654</v>
+        <v>0.6801689867974033</v>
       </c>
       <c r="E8" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9">
@@ -622,10 +622,10 @@
         <v>-0.103184236224579</v>
       </c>
       <c r="D9" t="n">
-        <v>1.017601270718214</v>
+        <v>1.203776511402847</v>
       </c>
       <c r="E9" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10">
@@ -643,10 +643,10 @@
         <v>0.1706255170149478</v>
       </c>
       <c r="D10" t="n">
-        <v>1.017601270718214</v>
+        <v>1.203776511402847</v>
       </c>
       <c r="E10" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11">
@@ -664,10 +664,10 @@
         <v>-0.5332984795482612</v>
       </c>
       <c r="D11" t="n">
-        <v>1.017601270718214</v>
+        <v>1.203776511402847</v>
       </c>
       <c r="E11" t="n">
-        <v>-6</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="12">
@@ -685,10 +685,10 @@
         <v>-0.3801473000784792</v>
       </c>
       <c r="D12" t="n">
-        <v>1.017601270718214</v>
+        <v>1.203776511402847</v>
       </c>
       <c r="E12" t="n">
-        <v>-2</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="13">
@@ -706,10 +706,10 @@
         <v>0.3548213752590765</v>
       </c>
       <c r="D13" t="n">
-        <v>0.6985867718348771</v>
+        <v>0.8671147665260216</v>
       </c>
       <c r="E13" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14">
@@ -727,10 +727,10 @@
         <v>0.03170675112282921</v>
       </c>
       <c r="D14" t="n">
-        <v>0.6985867718348771</v>
+        <v>0.8671147665260216</v>
       </c>
       <c r="E14" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15">
@@ -748,10 +748,10 @@
         <v>-0.3263965845951407</v>
       </c>
       <c r="D15" t="n">
-        <v>0.6985867718348771</v>
+        <v>0.8671147665260216</v>
       </c>
       <c r="E15" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16">
@@ -769,7 +769,7 @@
         <v>-0.2129219972196277</v>
       </c>
       <c r="D16" t="n">
-        <v>0.6985867718348771</v>
+        <v>0.8671147665260216</v>
       </c>
       <c r="E16" t="n">
         <v>5</v>
@@ -790,10 +790,10 @@
         <v>-0.2359642397169768</v>
       </c>
       <c r="D17" t="n">
-        <v>0.6985867718348771</v>
+        <v>0.8671147665260216</v>
       </c>
       <c r="E17" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18">
@@ -804,17 +804,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>-inf~1478.0</t>
+          <t>-inf~1478.2</t>
         </is>
       </c>
       <c r="C18" t="n">
         <v>-0.3644757635312008</v>
       </c>
       <c r="D18" t="n">
-        <v>0.3462574186266055</v>
+        <v>0.3278768552024591</v>
       </c>
       <c r="E18" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19">
@@ -825,14 +825,14 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>1478.0~2083.0</t>
+          <t>1478.2~2083.0</t>
         </is>
       </c>
       <c r="C19" t="n">
         <v>-0.09085362376848929</v>
       </c>
       <c r="D19" t="n">
-        <v>0.3462574186266055</v>
+        <v>0.3278768552024591</v>
       </c>
       <c r="E19" t="n">
         <v>9</v>
@@ -846,14 +846,14 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2083.0~3291.0</t>
+          <t>2083.0~3290.6</t>
         </is>
       </c>
       <c r="C20" t="n">
         <v>0.1155583406231092</v>
       </c>
       <c r="D20" t="n">
-        <v>0.3462574186266055</v>
+        <v>0.3278768552024591</v>
       </c>
       <c r="E20" t="n">
         <v>11</v>
@@ -867,17 +867,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>3291.0~inf</t>
+          <t>3290.6~inf</t>
         </is>
       </c>
       <c r="C21" t="n">
         <v>0.4717144936113016</v>
       </c>
       <c r="D21" t="n">
-        <v>0.3462574186266055</v>
+        <v>0.3278768552024591</v>
       </c>
       <c r="E21" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22">
@@ -895,10 +895,10 @@
         <v>0.3076673648049328</v>
       </c>
       <c r="D22" t="n">
-        <v>0.8575600783933367</v>
+        <v>0.968917714042864</v>
       </c>
       <c r="E22" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23">
@@ -916,10 +916,10 @@
         <v>-1.599868461023673</v>
       </c>
       <c r="D23" t="n">
-        <v>0.8575600783933367</v>
+        <v>0.968917714042864</v>
       </c>
       <c r="E23" t="n">
-        <v>-30</v>
+        <v>-35</v>
       </c>
     </row>
     <row r="24">
@@ -937,10 +937,10 @@
         <v>0.5423242907815011</v>
       </c>
       <c r="D24" t="n">
-        <v>0.8575600783933367</v>
+        <v>0.968917714042864</v>
       </c>
       <c r="E24" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25">
@@ -958,10 +958,10 @@
         <v>-0.6690496288880857</v>
       </c>
       <c r="D25" t="n">
-        <v>0.8575600783933367</v>
+        <v>0.968917714042864</v>
       </c>
       <c r="E25" t="n">
-        <v>-7</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="26">
@@ -979,10 +979,10 @@
         <v>-0.08239953175904276</v>
       </c>
       <c r="D26" t="n">
-        <v>0.8575600783933367</v>
+        <v>0.968917714042864</v>
       </c>
       <c r="E26" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27">
@@ -1000,10 +1000,10 @@
         <v>0.1996130538853391</v>
       </c>
       <c r="D27" t="n">
-        <v>0.8575600783933367</v>
+        <v>0.968917714042864</v>
       </c>
       <c r="E27" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28">
@@ -1021,7 +1021,7 @@
         <v>-0.0569259367905471</v>
       </c>
       <c r="D28" t="n">
-        <v>0.8575600783933367</v>
+        <v>0.968917714042864</v>
       </c>
       <c r="E28" t="n">
         <v>8</v>
@@ -1042,10 +1042,10 @@
         <v>-0.2388919082557814</v>
       </c>
       <c r="D29" t="n">
-        <v>0.8575600783933367</v>
+        <v>0.968917714042864</v>
       </c>
       <c r="E29" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30">
@@ -1063,10 +1063,10 @@
         <v>0.2578291092734902</v>
       </c>
       <c r="D30" t="n">
-        <v>0.8575600783933367</v>
+        <v>0.968917714042864</v>
       </c>
       <c r="E30" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31">
@@ -1084,7 +1084,7 @@
         <v>-0.1732717212562543</v>
       </c>
       <c r="D31" t="n">
-        <v>0.8575600783933367</v>
+        <v>0.968917714042864</v>
       </c>
       <c r="E31" t="n">
         <v>5</v>
@@ -1105,10 +1105,10 @@
         <v>0.4626235219051937</v>
       </c>
       <c r="D32" t="n">
-        <v>0.8575600783933367</v>
+        <v>0.968917714042864</v>
       </c>
       <c r="E32" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33">
@@ -1126,10 +1126,10 @@
         <v>0.3835823968254996</v>
       </c>
       <c r="D33" t="n">
-        <v>0.8575600783933367</v>
+        <v>0.968917714042864</v>
       </c>
       <c r="E33" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34">
@@ -1147,10 +1147,10 @@
         <v>0.4956162050614946</v>
       </c>
       <c r="D34" t="n">
-        <v>0.8575600783933367</v>
+        <v>0.968917714042864</v>
       </c>
       <c r="E34" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35">
@@ -1168,10 +1168,10 @@
         <v>-0.5447271753712584</v>
       </c>
       <c r="D35" t="n">
-        <v>0.8575600783933367</v>
+        <v>0.968917714042864</v>
       </c>
       <c r="E35" t="n">
-        <v>-4</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="36">
@@ -1189,10 +1189,10 @@
         <v>-0.4723593428779349</v>
       </c>
       <c r="D36" t="n">
-        <v>0.3150498778763671</v>
+        <v>0.2097011075286264</v>
       </c>
       <c r="E36" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37">
@@ -1210,10 +1210,10 @@
         <v>-0.1116399711312105</v>
       </c>
       <c r="D37" t="n">
-        <v>0.3150498778763671</v>
+        <v>0.2097011075286264</v>
       </c>
       <c r="E37" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38">
@@ -1231,10 +1231,10 @@
         <v>0.3427267674453865</v>
       </c>
       <c r="D38" t="n">
-        <v>0.3150498778763671</v>
+        <v>0.2097011075286264</v>
       </c>
       <c r="E38" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39">
@@ -1252,10 +1252,10 @@
         <v>2.178532444218721</v>
       </c>
       <c r="D39" t="n">
-        <v>0.3150498778763671</v>
+        <v>0.2097011075286264</v>
       </c>
       <c r="E39" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40">
@@ -1273,10 +1273,10 @@
         <v>0.872940290939283</v>
       </c>
       <c r="D40" t="n">
-        <v>0.3150498778763671</v>
+        <v>0.2097011075286264</v>
       </c>
       <c r="E40" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41">
@@ -1294,10 +1294,10 @@
         <v>1.684006607846946</v>
       </c>
       <c r="D41" t="n">
-        <v>0.3150498778763671</v>
+        <v>0.2097011075286264</v>
       </c>
       <c r="E41" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42">
@@ -1315,10 +1315,10 @@
         <v>0.1938937651975011</v>
       </c>
       <c r="D42" t="n">
-        <v>0.4840108169759975</v>
+        <v>0.6510072344208861</v>
       </c>
       <c r="E42" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43">
@@ -1336,10 +1336,10 @@
         <v>-0.2451224580056419</v>
       </c>
       <c r="D43" t="n">
-        <v>0.4840108169759975</v>
+        <v>0.6510072344208861</v>
       </c>
       <c r="E43" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44">
@@ -1357,10 +1357,10 @@
         <v>-0.2076393647553691</v>
       </c>
       <c r="D44" t="n">
-        <v>0.4840108169759975</v>
+        <v>0.6510072344208861</v>
       </c>
       <c r="E44" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45">
@@ -1378,10 +1378,10 @@
         <v>-0.07275935427663556</v>
       </c>
       <c r="D45" t="n">
-        <v>0.4840108169759975</v>
+        <v>0.6510072344208861</v>
       </c>
       <c r="E45" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46">
@@ -1399,178 +1399,178 @@
         <v>0.06595796778314181</v>
       </c>
       <c r="D46" t="n">
-        <v>0.4840108169759975</v>
+        <v>0.6510072344208861</v>
       </c>
       <c r="E46" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>appTimeAddress</t>
+          <t>cb90Ever</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>-0.001~-0.0</t>
+          <t>-inf~0.0</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>-0.1969982711884444</v>
+        <v>0.0868504888785427</v>
       </c>
       <c r="D47" t="n">
-        <v>0.1981395258591257</v>
+        <v>0.773555419898463</v>
       </c>
       <c r="E47" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>appTimeAddress</t>
+          <t>cb90Ever</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>-0.0~8.0</t>
+          <t>0.0~1.0</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>-0.001287830184428614</v>
+        <v>-0.3364722365815888</v>
       </c>
       <c r="D48" t="n">
-        <v>0.1981395258591257</v>
+        <v>0.773555419898463</v>
       </c>
       <c r="E48" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>appTimeAddress</t>
+          <t>cb90Ever</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>-inf~-0.001</t>
+          <t>1.0~inf</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>1.098612288551443</v>
+        <v>-0.09531017979482984</v>
       </c>
       <c r="D49" t="n">
-        <v>0.1981395258591257</v>
+        <v>0.773555419898463</v>
       </c>
       <c r="E49" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>appTimeAddress</t>
+          <t>cbFICO</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>13.0~inf</t>
+          <t>-0.001~628.0</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>0.03566018039505089</v>
+        <v>-0.5168122867547765</v>
       </c>
       <c r="D50" t="n">
-        <v>0.1981395258591257</v>
+        <v>0.8298702472100273</v>
       </c>
       <c r="E50" t="n">
-        <v>10</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>appTimeAddress</t>
+          <t>cbFICO</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>8.0~13.0</t>
+          <t>-inf~-0.001</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>0.2962658161166693</v>
+        <v>-0.3953127365966819</v>
       </c>
       <c r="D51" t="n">
-        <v>0.1981395258591257</v>
+        <v>0.8298702472100273</v>
       </c>
       <c r="E51" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>cb90Ever</t>
+          <t>cbFICO</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>-inf~0.0</t>
+          <t>628.0~669.0</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>0.0868504888785427</v>
+        <v>-0.097317205054122</v>
       </c>
       <c r="D52" t="n">
-        <v>0.5879477092517724</v>
+        <v>0.8298702472100273</v>
       </c>
       <c r="E52" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>cb90Ever</t>
+          <t>cbFICO</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>0.0~1.0</t>
+          <t>669.0~700.0</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>-0.3364722365815888</v>
+        <v>0.3315053389640824</v>
       </c>
       <c r="D53" t="n">
-        <v>0.5879477092517724</v>
+        <v>0.8298702472100273</v>
       </c>
       <c r="E53" t="n">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>cb90Ever</t>
+          <t>cbFICO</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>1.0~inf</t>
+          <t>700.0~725.0</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>-0.09531017979482984</v>
+        <v>0.9001613498829217</v>
       </c>
       <c r="D54" t="n">
-        <v>0.5879477092517724</v>
+        <v>0.8298702472100273</v>
       </c>
       <c r="E54" t="n">
-        <v>8</v>
+        <v>32</v>
       </c>
     </row>
     <row r="55">
@@ -1581,122 +1581,122 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>-0.001~628.0</t>
+          <t>725.0~inf</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>-0.5168122867547765</v>
+        <v>1.627787051020081</v>
       </c>
       <c r="D55" t="n">
-        <v>0.7490843771451504</v>
+        <v>0.8298702472100273</v>
       </c>
       <c r="E55" t="n">
-        <v>-2</v>
+        <v>49</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>cbFICO</t>
+          <t>cbInq5Mos</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>-inf~-0.001</t>
+          <t>-0.001~1.0</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>-0.3953127365966819</v>
+        <v>0.6359887666723824</v>
       </c>
       <c r="D56" t="n">
-        <v>0.7490843771451504</v>
+        <v>1.077128861841902</v>
       </c>
       <c r="E56" t="n">
-        <v>1</v>
+        <v>30</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>cbFICO</t>
+          <t>cbInq5Mos</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>628.0~669.0</t>
+          <t>-inf~-0.001</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>-0.097317205054122</v>
+        <v>0.154150679796306</v>
       </c>
       <c r="D57" t="n">
-        <v>0.7490843771451504</v>
+        <v>1.077128861841902</v>
       </c>
       <c r="E57" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>cbFICO</t>
+          <t>cbInq5Mos</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>669.0~700.0</t>
+          <t>1.0~3.0</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>0.3315053389640824</v>
+        <v>0.1893329790142457</v>
       </c>
       <c r="D58" t="n">
-        <v>0.7490843771451504</v>
+        <v>1.077128861841902</v>
       </c>
       <c r="E58" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>cbFICO</t>
+          <t>cbInq5Mos</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>700.0~725.0</t>
+          <t>16.0~17.0</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>0.9001613498829217</v>
+        <v>-2.484906648696334</v>
       </c>
       <c r="D59" t="n">
-        <v>0.7490843771451504</v>
+        <v>1.077128861841902</v>
       </c>
       <c r="E59" t="n">
-        <v>29</v>
+        <v>-67</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>cbFICO</t>
+          <t>cbInq5Mos</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>725.0~inf</t>
+          <t>17.0~inf</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>1.627787051020081</v>
+        <v>-0.5753641448289091</v>
       </c>
       <c r="D60" t="n">
-        <v>0.7490843771451504</v>
+        <v>1.077128861841902</v>
       </c>
       <c r="E60" t="n">
-        <v>45</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="61">
@@ -1707,17 +1707,17 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>-0.001~1.0</t>
+          <t>3.0~7.0</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>0.6359887666723824</v>
+        <v>-0.1729416026454343</v>
       </c>
       <c r="D61" t="n">
-        <v>0.9640510701576078</v>
+        <v>1.077128861841902</v>
       </c>
       <c r="E61" t="n">
-        <v>27</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62">
@@ -1728,122 +1728,122 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>-inf~-0.001</t>
+          <t>7.0~16.0</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>0.154150679796306</v>
+        <v>-0.4941932236532457</v>
       </c>
       <c r="D62" t="n">
-        <v>0.9640510701576078</v>
+        <v>1.077128861841902</v>
       </c>
       <c r="E62" t="n">
-        <v>14</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>cbInq5Mos</t>
+          <t>cbMosAvg</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>1.0~3.0</t>
+          <t>-0.001~-0.0</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>0.1893329790142457</v>
+        <v>0.3629054936526839</v>
       </c>
       <c r="D63" t="n">
-        <v>0.9640510701576078</v>
+        <v>0.865552592804646</v>
       </c>
       <c r="E63" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>cbInq5Mos</t>
+          <t>cbMosAvg</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>16.0~17.0</t>
+          <t>-0.0~6.0</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>-2.484906648696334</v>
+        <v>0.3596905266926738</v>
       </c>
       <c r="D64" t="n">
-        <v>0.9640510701576078</v>
+        <v>0.865552592804646</v>
       </c>
       <c r="E64" t="n">
-        <v>-60</v>
+        <v>19</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>cbInq5Mos</t>
+          <t>cbMosAvg</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>17.0~inf</t>
+          <t>-inf~-0.001</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>-0.5753641448289091</v>
+        <v>-0.1400792515807443</v>
       </c>
       <c r="D65" t="n">
-        <v>0.9640510701576078</v>
+        <v>0.865552592804646</v>
       </c>
       <c r="E65" t="n">
-        <v>-7</v>
+        <v>7</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>cbInq5Mos</t>
+          <t>cbMosAvg</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>3.0~7.0</t>
+          <t>33.0~34.0</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>-0.1729416026454343</v>
+        <v>1.791759469044722</v>
       </c>
       <c r="D66" t="n">
-        <v>0.9640510701576078</v>
+        <v>0.865552592804646</v>
       </c>
       <c r="E66" t="n">
-        <v>5</v>
+        <v>55</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>cbInq5Mos</t>
+          <t>cbMosAvg</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>7.0~16.0</t>
+          <t>34.0~inf</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>-0.4941932236532457</v>
+        <v>-0.3395071402766989</v>
       </c>
       <c r="D67" t="n">
-        <v>0.9640510701576078</v>
+        <v>0.865552592804646</v>
       </c>
       <c r="E67" t="n">
-        <v>-4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68">
@@ -1854,119 +1854,119 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>-0.001~-0.0</t>
+          <t>6.0~33.0</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>0.3629054936526839</v>
+        <v>-3.773648060701619e-13</v>
       </c>
       <c r="D68" t="n">
-        <v>0.6858899761932447</v>
+        <v>0.865552592804646</v>
       </c>
       <c r="E68" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>cbMosAvg</t>
+          <t>cbMosDlq</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>-0.0~6.0</t>
+          <t>-0.001~-0.0</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>0.3596905266926738</v>
+        <v>-0.4855078157230469</v>
       </c>
       <c r="D69" t="n">
-        <v>0.6858899761932447</v>
+        <v>0.831694226487085</v>
       </c>
       <c r="E69" t="n">
-        <v>17</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>cbMosAvg</t>
+          <t>cbMosDlq</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>-inf~-0.001</t>
+          <t>-0.0~4.0</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>-0.1400792515807443</v>
+        <v>-0.3570580122784784</v>
       </c>
       <c r="D70" t="n">
-        <v>0.6858899761932447</v>
+        <v>0.831694226487085</v>
       </c>
       <c r="E70" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>cbMosAvg</t>
+          <t>cbMosDlq</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>33.0~34.0</t>
+          <t>-inf~-0.001</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>1.791759469044722</v>
+        <v>0.1580392135521808</v>
       </c>
       <c r="D71" t="n">
-        <v>0.6858899761932447</v>
+        <v>0.831694226487085</v>
       </c>
       <c r="E71" t="n">
-        <v>45</v>
+        <v>14</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>cbMosAvg</t>
+          <t>cbMosDlq</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>34.0~inf</t>
+          <t>39.0~42.0</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>-0.3395071402766989</v>
+        <v>1.540445040835244</v>
       </c>
       <c r="D72" t="n">
-        <v>0.6858899761932447</v>
+        <v>0.831694226487085</v>
       </c>
       <c r="E72" t="n">
-        <v>3</v>
+        <v>47</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>cbMosAvg</t>
+          <t>cbMosDlq</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>6.0~33.0</t>
+          <t>4.0~39.0</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>-3.773648060701619e-13</v>
+        <v>-0.05794724404002055</v>
       </c>
       <c r="D73" t="n">
-        <v>0.6858899761932447</v>
+        <v>0.831694226487085</v>
       </c>
       <c r="E73" t="n">
         <v>9</v>
@@ -1980,17 +1980,17 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>-0.001~-0.0</t>
+          <t>42.0~63.0</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>-0.4855078157230469</v>
+        <v>0.02247285584756374</v>
       </c>
       <c r="D74" t="n">
-        <v>0.7291078600273293</v>
+        <v>0.831694226487085</v>
       </c>
       <c r="E74" t="n">
-        <v>-1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="75">
@@ -2001,206 +2001,206 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>-0.0~4.0</t>
+          <t>63.0~inf</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>-0.3570580122784784</v>
+        <v>0.6190392083553078</v>
       </c>
       <c r="D75" t="n">
-        <v>0.7291078600273293</v>
+        <v>0.831694226487085</v>
       </c>
       <c r="E75" t="n">
-        <v>2</v>
+        <v>25</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>cbMosDlq</t>
+          <t>cbMosInq</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>-inf~-0.001</t>
+          <t>-0.001~-0.0</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>0.1580392135521808</v>
+        <v>-0.06484113877586589</v>
       </c>
       <c r="D76" t="n">
-        <v>0.7291078600273293</v>
+        <v>0.4105290308013701</v>
       </c>
       <c r="E76" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>cbMosDlq</t>
+          <t>cbMosInq</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>39.0~42.0</t>
+          <t>-0.0~7.0</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>1.540445040835244</v>
+        <v>0.1859645480547562</v>
       </c>
       <c r="D77" t="n">
-        <v>0.7291078600273293</v>
+        <v>0.4105290308013701</v>
       </c>
       <c r="E77" t="n">
-        <v>42</v>
+        <v>12</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>cbMosDlq</t>
+          <t>cbMosInq</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>4.0~39.0</t>
+          <t>-inf~-0.001</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>-0.05794724404002055</v>
+        <v>0.7062192620740172</v>
       </c>
       <c r="D78" t="n">
-        <v>0.7291078600273293</v>
+        <v>0.4105290308013701</v>
       </c>
       <c r="E78" t="n">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>cbMosDlq</t>
+          <t>cbMosInq</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>42.0~63.0</t>
+          <t>7.0~inf</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>0.02247285584756374</v>
+        <v>1.845826690380787</v>
       </c>
       <c r="D79" t="n">
-        <v>0.7291078600273293</v>
+        <v>0.4105290308013701</v>
       </c>
       <c r="E79" t="n">
-        <v>10</v>
+        <v>32</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>cbMosDlq</t>
+          <t>cbPctGood</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>63.0~inf</t>
+          <t>-0.001~83.0</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>0.6190392083553078</v>
+        <v>-0.2386259154357761</v>
       </c>
       <c r="D80" t="n">
-        <v>0.7291078600273293</v>
+        <v>0.2369831906242948</v>
       </c>
       <c r="E80" t="n">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>cbMosInq</t>
+          <t>cbPctGood</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>-0.001~-0.0</t>
+          <t>-inf~-0.001</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>-0.06484113877586589</v>
+        <v>-0.3920420877293751</v>
       </c>
       <c r="D81" t="n">
-        <v>0.3039394055372003</v>
+        <v>0.2369831906242948</v>
       </c>
       <c r="E81" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>cbMosInq</t>
+          <t>cbPctGood</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>-0.0~7.0</t>
+          <t>83.0~85.0</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>0.1859645480547562</v>
+        <v>0.6286086593632075</v>
       </c>
       <c r="D82" t="n">
-        <v>0.3039394055372003</v>
+        <v>0.2369831906242948</v>
       </c>
       <c r="E82" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>cbMosInq</t>
+          <t>cbPctGood</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>-inf~-0.001</t>
+          <t>85.0~88.0</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>0.7062192620740172</v>
+        <v>-0.2564295289196363</v>
       </c>
       <c r="D83" t="n">
-        <v>0.3039394055372003</v>
+        <v>0.2369831906242948</v>
       </c>
       <c r="E83" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>cbMosInq</t>
+          <t>cbPctGood</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>7.0~inf</t>
+          <t>88.0~93.0</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>1.845826690380787</v>
+        <v>0.30228087184567</v>
       </c>
       <c r="D84" t="n">
-        <v>0.3039394055372003</v>
+        <v>0.2369831906242948</v>
       </c>
       <c r="E84" t="n">
-        <v>26</v>
+        <v>12</v>
       </c>
     </row>
     <row r="85">
@@ -2211,17 +2211,17 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>-0.001~83.0</t>
+          <t>93.0~96.0</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>-0.2386259154357761</v>
+        <v>0.9075570518414035</v>
       </c>
       <c r="D85" t="n">
-        <v>0.2745083842340353</v>
+        <v>0.2369831906242948</v>
       </c>
       <c r="E85" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="86">
@@ -2232,122 +2232,122 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>-inf~-0.001</t>
+          <t>96.0~inf</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>-0.3920420877293751</v>
+        <v>0.2176382286991</v>
       </c>
       <c r="D86" t="n">
-        <v>0.2745083842340353</v>
+        <v>0.2369831906242948</v>
       </c>
       <c r="E86" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>cbPctGood</t>
+          <t>cbTimeFile</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>83.0~85.0</t>
+          <t>-0.001~0.0</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>0.6286086593632075</v>
+        <v>-0.2876820724246974</v>
       </c>
       <c r="D87" t="n">
-        <v>0.2745083842340353</v>
+        <v>0.2058388364351974</v>
       </c>
       <c r="E87" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>cbPctGood</t>
+          <t>cbTimeFile</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>85.0~88.0</t>
+          <t>-inf~-0.001</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>-0.2564295289196363</v>
+        <v>0.06899287147314187</v>
       </c>
       <c r="D88" t="n">
-        <v>0.2745083842340353</v>
+        <v>0.2058388364351974</v>
       </c>
       <c r="E88" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>cbPctGood</t>
+          <t>cbTimeFile</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>88.0~93.0</t>
+          <t>0.0~22.0</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>0.30228087184567</v>
+        <v>-0.6443570163004536</v>
       </c>
       <c r="D89" t="n">
-        <v>0.2745083842340353</v>
+        <v>0.2058388364351974</v>
       </c>
       <c r="E89" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>cbPctGood</t>
+          <t>cbTimeFile</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>93.0~96.0</t>
+          <t>164.0~inf</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>0.9075570518414035</v>
+        <v>0.8174448971809433</v>
       </c>
       <c r="D90" t="n">
-        <v>0.2745083842340353</v>
+        <v>0.2058388364351974</v>
       </c>
       <c r="E90" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>cbPctGood</t>
+          <t>cbTimeFile</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>96.0~inf</t>
+          <t>22.0~79.0</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>0.2176382286991</v>
+        <v>-0.2551829050299068</v>
       </c>
       <c r="D91" t="n">
-        <v>0.2745083842340353</v>
+        <v>0.2058388364351974</v>
       </c>
       <c r="E91" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="92">
@@ -2358,122 +2358,122 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>-0.001~0.0</t>
+          <t>79.0~164.0</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>-0.2876820724246974</v>
+        <v>0.2004582684647281</v>
       </c>
       <c r="D92" t="n">
-        <v>0.1969307689617434</v>
+        <v>0.2058388364351974</v>
       </c>
       <c r="E92" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>cbTimeFile</t>
+          <t>cbTimeFileYears</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>-inf~-0.001</t>
+          <t>-0.001~4.0</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>0.06899287147314187</v>
+        <v>-0.4184804761684133</v>
       </c>
       <c r="D93" t="n">
-        <v>0.1969307689617434</v>
+        <v>0.05383133952900197</v>
       </c>
       <c r="E93" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>cbTimeFile</t>
+          <t>cbTimeFileYears</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>0.0~22.0</t>
+          <t>-inf~-0.001</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>-0.6443570163004536</v>
+        <v>0.06899287147314187</v>
       </c>
       <c r="D94" t="n">
-        <v>0.1969307689617434</v>
+        <v>0.05383133952900197</v>
       </c>
       <c r="E94" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>cbTimeFile</t>
+          <t>cbTimeFileYears</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>164.0~inf</t>
+          <t>14.0~27.0</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>0.8174448971809433</v>
+        <v>0.9354606479200405</v>
       </c>
       <c r="D95" t="n">
-        <v>0.1969307689617434</v>
+        <v>0.05383133952900197</v>
       </c>
       <c r="E95" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>cbTimeFile</t>
+          <t>cbTimeFileYears</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>22.0~79.0</t>
+          <t>27.0~29.0</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>-0.2551829050299068</v>
+        <v>-0.2876820724309475</v>
       </c>
       <c r="D96" t="n">
-        <v>0.1969307689617434</v>
+        <v>0.05383133952900197</v>
       </c>
       <c r="E96" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>cbTimeFile</t>
+          <t>cbTimeFileYears</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>79.0~164.0</t>
+          <t>29.0~inf</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>0.2004582684647281</v>
+        <v>0.9985288300336835</v>
       </c>
       <c r="D97" t="n">
-        <v>0.1969307689617434</v>
+        <v>0.05383133952900197</v>
       </c>
       <c r="E97" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="98">
@@ -2484,17 +2484,17 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>-0.001~4.0</t>
+          <t>4.0~7.0</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>-0.4184804761684133</v>
+        <v>-0.05437677087276212</v>
       </c>
       <c r="D98" t="n">
-        <v>0.120573776272358</v>
+        <v>0.05383133952900197</v>
       </c>
       <c r="E98" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="99">
@@ -2505,35 +2505,35 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>-inf~-0.001</t>
+          <t>7.0~14.0</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>0.06899287147314187</v>
+        <v>0.2744368456774507</v>
       </c>
       <c r="D99" t="n">
-        <v>0.120573776272358</v>
+        <v>0.05383133952900197</v>
       </c>
       <c r="E99" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>cbTimeFileYears</t>
+          <t>cbUtilizn</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>14.0~27.0</t>
+          <t>-0.001~-0.0</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>0.9354606479200405</v>
+        <v>0.1488456275825007</v>
       </c>
       <c r="D100" t="n">
-        <v>0.120573776272358</v>
+        <v>0.7833239214969772</v>
       </c>
       <c r="E100" t="n">
         <v>13</v>
@@ -2542,85 +2542,85 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>cbTimeFileYears</t>
+          <t>cbUtilizn</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>27.0~29.0</t>
+          <t>-0.0~5.0</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>-0.2876820724309475</v>
+        <v>1.429466532903161</v>
       </c>
       <c r="D101" t="n">
-        <v>0.120573776272358</v>
+        <v>0.7833239214969772</v>
       </c>
       <c r="E101" t="n">
-        <v>8</v>
+        <v>42</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>cbTimeFileYears</t>
+          <t>cbUtilizn</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>29.0~inf</t>
+          <t>-inf~-0.001</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>0.9985288300336835</v>
+        <v>-0.4449439190261266</v>
       </c>
       <c r="D102" t="n">
-        <v>0.120573776272358</v>
+        <v>0.7833239214969772</v>
       </c>
       <c r="E102" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>cbTimeFileYears</t>
+          <t>cbUtilizn</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>4.0~7.0</t>
+          <t>16.0~61.0</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>-0.05437677087276212</v>
+        <v>0.2927126256148327</v>
       </c>
       <c r="D103" t="n">
-        <v>0.120573776272358</v>
+        <v>0.7833239214969772</v>
       </c>
       <c r="E103" t="n">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>cbTimeFileYears</t>
+          <t>cbUtilizn</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>7.0~14.0</t>
+          <t>5.0~16.0</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>0.2744368456774507</v>
+        <v>0.733969175026117</v>
       </c>
       <c r="D104" t="n">
-        <v>0.120573776272358</v>
+        <v>0.7833239214969772</v>
       </c>
       <c r="E104" t="n">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
     <row r="105">
@@ -2631,17 +2631,17 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>-0.001~-0.0</t>
+          <t>61.0~93.0</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>0.1488456275825007</v>
+        <v>-0.01652930194981706</v>
       </c>
       <c r="D105" t="n">
-        <v>0.6891537830864554</v>
+        <v>0.7833239214969772</v>
       </c>
       <c r="E105" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="106">
@@ -2652,122 +2652,122 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>-0.0~5.0</t>
+          <t>93.0~inf</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>1.429466532903161</v>
+        <v>-0.4519851236864824</v>
       </c>
       <c r="D106" t="n">
-        <v>0.6891537830864554</v>
+        <v>0.7833239214969772</v>
       </c>
       <c r="E106" t="n">
-        <v>38</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>cbUtilizn</t>
+          <t>dealLoanToVal</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>-inf~-0.001</t>
+          <t>-inf~49.7</t>
         </is>
       </c>
       <c r="C107" t="n">
-        <v>-0.4449439190261266</v>
+        <v>1.754019141151405</v>
       </c>
       <c r="D107" t="n">
-        <v>0.6891537830864554</v>
+        <v>0.9846268466952749</v>
       </c>
       <c r="E107" t="n">
-        <v>1</v>
+        <v>60</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>cbUtilizn</t>
+          <t>dealLoanToVal</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>16.0~61.0</t>
+          <t>49.7~73.1</t>
         </is>
       </c>
       <c r="C108" t="n">
-        <v>0.2927126256148327</v>
+        <v>0.55852468030953</v>
       </c>
       <c r="D108" t="n">
-        <v>0.6891537830864554</v>
+        <v>0.9846268466952749</v>
       </c>
       <c r="E108" t="n">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>cbUtilizn</t>
+          <t>dealLoanToVal</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>5.0~16.0</t>
+          <t>73.1~83.1</t>
         </is>
       </c>
       <c r="C109" t="n">
-        <v>0.733969175026117</v>
+        <v>0.1078889620006413</v>
       </c>
       <c r="D109" t="n">
-        <v>0.6891537830864554</v>
+        <v>0.9846268466952749</v>
       </c>
       <c r="E109" t="n">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>cbUtilizn</t>
+          <t>dealLoanToVal</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>61.0~93.0</t>
+          <t>83.1~91.3</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>-0.01652930194981706</v>
+        <v>-0.2070594192540108</v>
       </c>
       <c r="D110" t="n">
-        <v>0.6891537830864554</v>
+        <v>0.9846268466952749</v>
       </c>
       <c r="E110" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>cbUtilizn</t>
+          <t>dealLoanToVal</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>93.0~inf</t>
+          <t>91.3~91.5</t>
         </is>
       </c>
       <c r="C111" t="n">
-        <v>-0.4519851236864824</v>
+        <v>0.6931471805008543</v>
       </c>
       <c r="D111" t="n">
-        <v>0.6891537830864554</v>
+        <v>0.9846268466952749</v>
       </c>
       <c r="E111" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="112">
@@ -2778,101 +2778,17 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>-inf~50.0</t>
+          <t>91.5~inf</t>
         </is>
       </c>
       <c r="C112" t="n">
-        <v>1.648658625496612</v>
+        <v>-0.1899179036652446</v>
       </c>
       <c r="D112" t="n">
-        <v>0.7073436180440542</v>
+        <v>0.9846268466952749</v>
       </c>
       <c r="E112" t="n">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="inlineStr">
-        <is>
-          <t>dealLoanToVal</t>
-        </is>
-      </c>
-      <c r="B113" t="inlineStr">
-        <is>
-          <t>50.0~68.0</t>
-        </is>
-      </c>
-      <c r="C113" t="n">
-        <v>0.6649763035432886</v>
-      </c>
-      <c r="D113" t="n">
-        <v>0.7073436180440542</v>
-      </c>
-      <c r="E113" t="n">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="inlineStr">
-        <is>
-          <t>dealLoanToVal</t>
-        </is>
-      </c>
-      <c r="B114" t="inlineStr">
-        <is>
-          <t>68.0~78.0</t>
-        </is>
-      </c>
-      <c r="C114" t="n">
-        <v>0.3162339743525008</v>
-      </c>
-      <c r="D114" t="n">
-        <v>0.7073436180440542</v>
-      </c>
-      <c r="E114" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" t="inlineStr">
-        <is>
-          <t>dealLoanToVal</t>
-        </is>
-      </c>
-      <c r="B115" t="inlineStr">
-        <is>
-          <t>78.0~83.0</t>
-        </is>
-      </c>
-      <c r="C115" t="n">
-        <v>0.02884815433432703</v>
-      </c>
-      <c r="D115" t="n">
-        <v>0.7073436180440542</v>
-      </c>
-      <c r="E115" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" t="inlineStr">
-        <is>
-          <t>dealLoanToVal</t>
-        </is>
-      </c>
-      <c r="B116" t="inlineStr">
-        <is>
-          <t>83.0~inf</t>
-        </is>
-      </c>
-      <c r="C116" t="n">
-        <v>-0.1848031844671148</v>
-      </c>
-      <c r="D116" t="n">
-        <v>0.7073436180440542</v>
-      </c>
-      <c r="E116" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chimerge, LR param testing
</commit_message>
<xml_diff>
--- a/hw2/scorecards/scorecards.xlsx
+++ b/hw2/scorecards/scorecards.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E130"/>
+  <dimension ref="A1:E98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,17 +468,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>-0.0~20.0</t>
+          <t>-0.001~18.0</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>-0.6167742016908709</v>
+        <v>-0.3101549282741426</v>
       </c>
       <c r="D2" t="n">
-        <v>0.6113626937271748</v>
+        <v>0.6129455539065072</v>
       </c>
       <c r="E2" t="n">
-        <v>-1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
@@ -493,10 +493,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.09531017979323402</v>
+        <v>0.1466034741764847</v>
       </c>
       <c r="D3" t="n">
-        <v>0.6113626937271748</v>
+        <v>0.6129455539065072</v>
       </c>
       <c r="E3" t="n">
         <v>12</v>
@@ -510,17 +510,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>20.0~37.0</t>
+          <t>18.0~22.0</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-0.09878766380773628</v>
+        <v>-0.5557049498694202</v>
       </c>
       <c r="D4" t="n">
-        <v>0.6113626937271748</v>
+        <v>0.6129455539065072</v>
       </c>
       <c r="E4" t="n">
-        <v>8</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="5">
@@ -531,17 +531,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>37.0~48.0</t>
+          <t>22.0~36.0</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.2449571277633332</v>
+        <v>-0.05446890835595959</v>
       </c>
       <c r="D5" t="n">
-        <v>0.6113626937271748</v>
+        <v>0.6129455539065072</v>
       </c>
       <c r="E5" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
@@ -552,38 +552,38 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>48.0~87.0</t>
+          <t>36.0~inf</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.3287435592209389</v>
+        <v>0.2857899242746959</v>
       </c>
       <c r="D6" t="n">
-        <v>0.6113626937271748</v>
+        <v>0.6129455539065072</v>
       </c>
       <c r="E6" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>appAge</t>
+          <t>appChkSv</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>87.0~inf</t>
+          <t>-inf~0.0</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-23.02585092994046</v>
+        <v>-0.1256552689349857</v>
       </c>
       <c r="D7" t="n">
-        <v>0.6113626937271748</v>
+        <v>1.163556541551396</v>
       </c>
       <c r="E7" t="n">
-        <v>-396</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8">
@@ -594,17 +594,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>-inf~0.0</t>
+          <t>0.0~1.0</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>-0.103184236224579</v>
+        <v>0.1772922083725946</v>
       </c>
       <c r="D8" t="n">
-        <v>1.317532877272823</v>
+        <v>1.163556541551396</v>
       </c>
       <c r="E8" t="n">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9">
@@ -615,17 +615,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>0.0~1.0</t>
+          <t>1.0~2.0</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.1706255170149478</v>
+        <v>-0.5089547157643856</v>
       </c>
       <c r="D9" t="n">
-        <v>1.317532877272823</v>
+        <v>1.163556541551396</v>
       </c>
       <c r="E9" t="n">
-        <v>16</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="10">
@@ -636,38 +636,38 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>1.0~2.0</t>
+          <t>2.0~inf</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>-0.5332984795482612</v>
+        <v>-0.3470543459110124</v>
       </c>
       <c r="D10" t="n">
-        <v>1.317532877272823</v>
+        <v>1.163556541551396</v>
       </c>
       <c r="E10" t="n">
-        <v>-10</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>appChkSv</t>
+          <t>appFinanceCo</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2.0~inf</t>
+          <t>-inf~0.0</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>-0.3801473000784792</v>
+        <v>0.3639653771704967</v>
       </c>
       <c r="D11" t="n">
-        <v>1.317532877272823</v>
+        <v>0.6419820113332315</v>
       </c>
       <c r="E11" t="n">
-        <v>-4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12">
@@ -678,17 +678,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>-inf~0.0</t>
+          <t>0.0~1.0</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.3548213752590765</v>
+        <v>0.04525659158358021</v>
       </c>
       <c r="D12" t="n">
-        <v>0.8354183252925764</v>
+        <v>0.6419820113332315</v>
       </c>
       <c r="E12" t="n">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13">
@@ -699,17 +699,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>0.0~1.0</t>
+          <t>1.0~2.0</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.03170675112282921</v>
+        <v>-0.3317773922788375</v>
       </c>
       <c r="D13" t="n">
-        <v>0.8354183252925764</v>
+        <v>0.6419820113332315</v>
       </c>
       <c r="E13" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14">
@@ -720,17 +720,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>1.0~2.0</t>
+          <t>2.0~3.0</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>-0.3263965845951407</v>
+        <v>-0.2432303098539789</v>
       </c>
       <c r="D14" t="n">
-        <v>0.8354183252925764</v>
+        <v>0.6419820113332315</v>
       </c>
       <c r="E14" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15">
@@ -741,14 +741,14 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2.0~3.0</t>
+          <t>3.0~inf</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>-0.2129219972196277</v>
+        <v>-0.2573635960362713</v>
       </c>
       <c r="D15" t="n">
-        <v>0.8354183252925764</v>
+        <v>0.6419820113332315</v>
       </c>
       <c r="E15" t="n">
         <v>5</v>
@@ -757,22 +757,22 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>appFinanceCo</t>
+          <t>appIncome</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>3.0~inf</t>
+          <t>-inf~1410.0</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-0.2359642397169768</v>
+        <v>-0.3481506514707269</v>
       </c>
       <c r="D16" t="n">
-        <v>0.8354183252925764</v>
+        <v>0.2635015802480362</v>
       </c>
       <c r="E16" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17">
@@ -783,17 +783,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>-inf~800.0</t>
+          <t>1410.0~2272.8</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-0.2559333741112598</v>
+        <v>-0.08763423592323295</v>
       </c>
       <c r="D17" t="n">
-        <v>0.5941401789702806</v>
+        <v>0.2635015802480362</v>
       </c>
       <c r="E17" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18">
@@ -804,17 +804,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>1620.0~1681.9</t>
+          <t>2272.8~3300.0</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.1082135846271192</v>
+        <v>0.1322216347298122</v>
       </c>
       <c r="D18" t="n">
-        <v>0.5941401789702806</v>
+        <v>0.2635015802480362</v>
       </c>
       <c r="E18" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19">
@@ -825,122 +825,122 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>1681.9~1700.0</t>
+          <t>3300.0~inf</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>-0.390866308642127</v>
+        <v>0.4749911707185637</v>
       </c>
       <c r="D19" t="n">
-        <v>0.5941401789702806</v>
+        <v>0.2635015802480362</v>
       </c>
       <c r="E19" t="n">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>appIncome</t>
+          <t>appOcc</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>1700.0~1733.0</t>
+          <t>-0.001~1.0</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>-0.8472978602610132</v>
+        <v>0.2422492103717739</v>
       </c>
       <c r="D20" t="n">
-        <v>0.5941401789702806</v>
+        <v>0.7892530617802295</v>
       </c>
       <c r="E20" t="n">
-        <v>-5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>appIncome</t>
+          <t>appOcc</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>1733.0~2800.0</t>
+          <t>-inf~-0.001</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>-2.057243264630627e-13</v>
+        <v>-1.643629276765829</v>
       </c>
       <c r="D21" t="n">
-        <v>0.5941401789702806</v>
+        <v>0.7892530617802295</v>
       </c>
       <c r="E21" t="n">
-        <v>10</v>
+        <v>-28</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>appIncome</t>
+          <t>appOcc</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2800.0~inf</t>
+          <t>1.0~2.0</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.3722795590911297</v>
+        <v>0.6161861393759651</v>
       </c>
       <c r="D22" t="n">
-        <v>0.5941401789702806</v>
+        <v>0.7892530617802295</v>
       </c>
       <c r="E22" t="n">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>appIncome</t>
+          <t>appOcc</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>800.0~900.0</t>
+          <t>10.0~11.0</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>-0.6931471804617971</v>
+        <v>-0.7137664676605552</v>
       </c>
       <c r="D23" t="n">
-        <v>0.5941401789702806</v>
+        <v>0.7892530617802295</v>
       </c>
       <c r="E23" t="n">
-        <v>-2</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>appIncome</t>
+          <t>appOcc</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>900.0~1620.0</t>
+          <t>11.0~12.0</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>-0.2260948569236171</v>
+        <v>-0.06618190687495157</v>
       </c>
       <c r="D24" t="n">
-        <v>0.5941401789702806</v>
+        <v>0.7892530617802295</v>
       </c>
       <c r="E24" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25">
@@ -951,17 +951,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>-0.001~1.0</t>
+          <t>12.0~inf</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.3076673648049328</v>
+        <v>0.1615706126735225</v>
       </c>
       <c r="D25" t="n">
-        <v>1.004414472221974</v>
+        <v>0.7892530617802295</v>
       </c>
       <c r="E25" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26">
@@ -972,17 +972,17 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>-inf~-0.001</t>
+          <t>2.0~3.0</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>-1.599868461023673</v>
+        <v>-0.05480823648969457</v>
       </c>
       <c r="D26" t="n">
-        <v>1.004414472221974</v>
+        <v>0.7892530617802295</v>
       </c>
       <c r="E26" t="n">
-        <v>-36</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27">
@@ -993,17 +993,17 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>1.0~2.0</t>
+          <t>3.0~4.0</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.5423242907815011</v>
+        <v>-0.1786109773782351</v>
       </c>
       <c r="D27" t="n">
-        <v>1.004414472221974</v>
+        <v>0.7892530617802295</v>
       </c>
       <c r="E27" t="n">
-        <v>26</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28">
@@ -1014,17 +1014,17 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>10.0~11.0</t>
+          <t>4.0~5.0</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>-0.6690496288880857</v>
+        <v>0.1335313926072608</v>
       </c>
       <c r="D28" t="n">
-        <v>1.004414472221974</v>
+        <v>0.7892530617802295</v>
       </c>
       <c r="E28" t="n">
-        <v>-9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29">
@@ -1035,17 +1035,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>11.0~12.0</t>
+          <t>5.0~6.0</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>-0.08239953175904276</v>
+        <v>-0.190518323978166</v>
       </c>
       <c r="D29" t="n">
-        <v>1.004414472221974</v>
+        <v>0.7892530617802295</v>
       </c>
       <c r="E29" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30">
@@ -1056,17 +1056,17 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>12.0~inf</t>
+          <t>6.0~7.0</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.1996130538853391</v>
+        <v>0.4519851237019317</v>
       </c>
       <c r="D30" t="n">
-        <v>1.004414472221974</v>
+        <v>0.7892530617802295</v>
       </c>
       <c r="E30" t="n">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31">
@@ -1077,17 +1077,17 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2.0~3.0</t>
+          <t>7.0~8.0</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>-0.0569259367905471</v>
+        <v>0.4092034301840659</v>
       </c>
       <c r="D31" t="n">
-        <v>1.004414472221974</v>
+        <v>0.7892530617802295</v>
       </c>
       <c r="E31" t="n">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32">
@@ -1098,17 +1098,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>3.0~4.0</t>
+          <t>8.0~9.0</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>-0.2388919082557814</v>
+        <v>0.5007752878714286</v>
       </c>
       <c r="D32" t="n">
-        <v>1.004414472221974</v>
+        <v>0.7892530617802295</v>
       </c>
       <c r="E32" t="n">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33">
@@ -1119,560 +1119,560 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>4.0~5.0</t>
+          <t>9.0~10.0</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.2578291092734902</v>
+        <v>-0.5511769192177236</v>
       </c>
       <c r="D33" t="n">
-        <v>1.004414472221974</v>
+        <v>0.7892530617802295</v>
       </c>
       <c r="E33" t="n">
-        <v>17</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>appOcc</t>
+          <t>appOrigScore</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>5.0~6.0</t>
+          <t>-inf~190.0</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>-0.1732717212562543</v>
+        <v>-0.5283436961216631</v>
       </c>
       <c r="D34" t="n">
-        <v>1.004414472221974</v>
+        <v>0.4051568746064499</v>
       </c>
       <c r="E34" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>appOcc</t>
+          <t>appOrigScore</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>6.0~7.0</t>
+          <t>190.0~203.0</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.4626235219051937</v>
+        <v>-0.1927074068050093</v>
       </c>
       <c r="D35" t="n">
-        <v>1.004414472221974</v>
+        <v>0.4051568746064499</v>
       </c>
       <c r="E35" t="n">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>appOcc</t>
+          <t>appOrigScore</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>7.0~8.0</t>
+          <t>203.0~219.0</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.3835823968254996</v>
+        <v>0.3525849586572027</v>
       </c>
       <c r="D36" t="n">
-        <v>1.004414472221974</v>
+        <v>0.4051568746064499</v>
       </c>
       <c r="E36" t="n">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>appOcc</t>
+          <t>appOrigScore</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>8.0~9.0</t>
+          <t>219.0~inf</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.4956162050614946</v>
+        <v>1.504077396697214</v>
       </c>
       <c r="D37" t="n">
-        <v>1.004414472221974</v>
+        <v>0.4051568746064499</v>
       </c>
       <c r="E37" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>appOcc</t>
+          <t>appResidence</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>9.0~10.0</t>
+          <t>-inf~0.0</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>-0.5447271753712584</v>
+        <v>0.205942188936922</v>
       </c>
       <c r="D38" t="n">
-        <v>1.004414472221974</v>
+        <v>0.4519662018680377</v>
       </c>
       <c r="E38" t="n">
-        <v>-6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>appOrigScore</t>
+          <t>appResidence</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>-inf~142.0</t>
+          <t>0.0~1.0</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>23.02585092984046</v>
+        <v>-0.2674312314850266</v>
       </c>
       <c r="D39" t="n">
-        <v>0.473498633184935</v>
+        <v>0.4519662018680377</v>
       </c>
       <c r="E39" t="n">
-        <v>325</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>appOrigScore</t>
+          <t>appResidence</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>142.0~160.0</t>
+          <t>1.0~2.0</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>-0.3513978867994869</v>
+        <v>-0.1983665469555332</v>
       </c>
       <c r="D40" t="n">
-        <v>0.473498633184935</v>
+        <v>0.4519662018680377</v>
       </c>
       <c r="E40" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>appOrigScore</t>
+          <t>appResidence</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>160.0~198.0</t>
+          <t>2.0~3.0</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>-0.4278032747020784</v>
+        <v>-0.07755823433930259</v>
       </c>
       <c r="D41" t="n">
-        <v>0.473498633184935</v>
+        <v>0.4519662018680377</v>
       </c>
       <c r="E41" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>appOrigScore</t>
+          <t>appResidence</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>198.0~203.0</t>
+          <t>3.0~inf</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>-0.1184816036085034</v>
+        <v>-0.0571584138359181</v>
       </c>
       <c r="D42" t="n">
-        <v>0.473498633184935</v>
+        <v>0.4519662018680377</v>
       </c>
       <c r="E42" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>appOrigScore</t>
+          <t>cb90Ever</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>203.0~215.0</t>
+          <t>-inf~0.0</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>0.278819385169211</v>
+        <v>0.08989500410786816</v>
       </c>
       <c r="D43" t="n">
-        <v>0.473498633184935</v>
+        <v>0.5432221669760897</v>
       </c>
       <c r="E43" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>appOrigScore</t>
+          <t>cb90Ever</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>215.0~220.0</t>
+          <t>0.0~1.0</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>0.8593825995424902</v>
+        <v>-0.3261695053993852</v>
       </c>
       <c r="D44" t="n">
-        <v>0.473498633184935</v>
+        <v>0.5432221669760897</v>
       </c>
       <c r="E44" t="n">
-        <v>22</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>appOrigScore</t>
+          <t>cb90Ever</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>220.0~223.0</t>
+          <t>1.0~8.0</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>1.679642171016902</v>
+        <v>-0.1556533096954015</v>
       </c>
       <c r="D45" t="n">
-        <v>0.473498633184935</v>
+        <v>0.5432221669760897</v>
       </c>
       <c r="E45" t="n">
-        <v>33</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>appOrigScore</t>
+          <t>cb90Ever</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>223.0~inf</t>
+          <t>8.0~inf</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>1.372042338336161</v>
+        <v>0.4519851236924078</v>
       </c>
       <c r="D46" t="n">
-        <v>0.473498633184935</v>
+        <v>0.5432221669760897</v>
       </c>
       <c r="E46" t="n">
-        <v>29</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>appResidence</t>
+          <t>cbFICO</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>-inf~0.0</t>
+          <t>-0.001~628.0</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.1938937651975011</v>
+        <v>-0.5336702563796119</v>
       </c>
       <c r="D47" t="n">
-        <v>0.7303460169290052</v>
+        <v>0.7634632658662862</v>
       </c>
       <c r="E47" t="n">
-        <v>14</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>appResidence</t>
+          <t>cbFICO</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>0.0~1.0</t>
+          <t>-inf~-0.001</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>-0.2451224580056419</v>
+        <v>-0.3667505958840474</v>
       </c>
       <c r="D48" t="n">
-        <v>0.7303460169290052</v>
+        <v>0.7634632658662862</v>
       </c>
       <c r="E48" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>appResidence</t>
+          <t>cbFICO</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>1.0~2.0</t>
+          <t>628.0~674.0</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>-0.2076393647553691</v>
+        <v>-0.05926146403082055</v>
       </c>
       <c r="D49" t="n">
-        <v>0.7303460169290052</v>
+        <v>0.7634632658662862</v>
       </c>
       <c r="E49" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>appResidence</t>
+          <t>cbFICO</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>2.0~3.0</t>
+          <t>674.0~725.0</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>-0.07275935427663556</v>
+        <v>0.5529178392083547</v>
       </c>
       <c r="D50" t="n">
-        <v>0.7303460169290052</v>
+        <v>0.7634632658662862</v>
       </c>
       <c r="E50" t="n">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>appResidence</t>
+          <t>cbFICO</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>3.0~inf</t>
+          <t>725.0~inf</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>0.06595796778314181</v>
+        <v>1.647417160416959</v>
       </c>
       <c r="D51" t="n">
-        <v>0.7303460169290052</v>
+        <v>0.7634632658662862</v>
       </c>
       <c r="E51" t="n">
-        <v>11</v>
+        <v>46</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>cb90Ever</t>
+          <t>cbInq5Mos</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>-inf~0.0</t>
+          <t>-0.001~1.0</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>0.0868504888785427</v>
+        <v>0.6491302950949425</v>
       </c>
       <c r="D52" t="n">
-        <v>0.8203970478977428</v>
+        <v>0.9627965626594224</v>
       </c>
       <c r="E52" t="n">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>cb90Ever</t>
+          <t>cbInq5Mos</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>0.0~1.0</t>
+          <t>-inf~-0.001</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>-0.3364722365815888</v>
+        <v>-0.3566749439058752</v>
       </c>
       <c r="D53" t="n">
-        <v>0.8203970478977428</v>
+        <v>0.9627965626594224</v>
       </c>
       <c r="E53" t="n">
-        <v>2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>cb90Ever</t>
+          <t>cbInq5Mos</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>1.0~6.0</t>
+          <t>1.0~2.0</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>-0.1144103511661635</v>
+        <v>0.2607262624398763</v>
       </c>
       <c r="D54" t="n">
-        <v>0.8203970478977428</v>
+        <v>0.9627965626594224</v>
       </c>
       <c r="E54" t="n">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>cb90Ever</t>
+          <t>cbInq5Mos</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>10.0~inf</t>
+          <t>2.0~5.0</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>-0.2876820724434476</v>
+        <v>-0.0449513878578257</v>
       </c>
       <c r="D55" t="n">
-        <v>0.8203970478977428</v>
+        <v>0.9627965626594224</v>
       </c>
       <c r="E55" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>cb90Ever</t>
+          <t>cbInq5Mos</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>6.0~10.0</t>
+          <t>5.0~inf</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>0.2876820724156697</v>
+        <v>-0.429266615521029</v>
       </c>
       <c r="D56" t="n">
-        <v>0.8203970478977428</v>
+        <v>0.9627965626594224</v>
       </c>
       <c r="E56" t="n">
-        <v>17</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>cbFICO</t>
+          <t>cbMosAvg</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>-0.001~542.0</t>
+          <t>-0.001~-0.0</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>-0.4818380868318141</v>
+        <v>0.4248831939247683</v>
       </c>
       <c r="D57" t="n">
-        <v>0.3743913316864461</v>
+        <v>0.7690931475806985</v>
       </c>
       <c r="E57" t="n">
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>cbFICO</t>
+          <t>cbMosAvg</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>-inf~-0.001</t>
+          <t>-0.0~4.0</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>-0.3953127365966819</v>
+        <v>0.3960310758417523</v>
       </c>
       <c r="D58" t="n">
-        <v>0.3743913316864461</v>
+        <v>0.7690931475806985</v>
       </c>
       <c r="E58" t="n">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>cbFICO</t>
+          <t>cbMosAvg</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>542.0~660.0</t>
+          <t>-inf~-0.001</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>-0.3411942887118533</v>
+        <v>-0.1543299073405065</v>
       </c>
       <c r="D59" t="n">
-        <v>0.3743913316864461</v>
+        <v>0.7690931475806985</v>
       </c>
       <c r="E59" t="n">
         <v>6</v>
@@ -1681,19 +1681,19 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>cbFICO</t>
+          <t>cbMosAvg</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>660.0~676.0</t>
+          <t>4.0~41.0</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>0.01574835696578287</v>
+        <v>0.05007005263967806</v>
       </c>
       <c r="D60" t="n">
-        <v>0.3743913316864461</v>
+        <v>0.7690931475806985</v>
       </c>
       <c r="E60" t="n">
         <v>10</v>
@@ -1702,229 +1702,229 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>cbFICO</t>
+          <t>cbMosAvg</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>676.0~680.0</t>
+          <t>41.0~inf</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>0.1053605156441227</v>
+        <v>-0.3829922522103482</v>
       </c>
       <c r="D61" t="n">
-        <v>0.3743913316864461</v>
+        <v>0.7690931475806985</v>
       </c>
       <c r="E61" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>cbFICO</t>
+          <t>cbMosDlq</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>680.0~707.0</t>
+          <t>-0.001~-0.0</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>0.4348397167519925</v>
+        <v>-0.4769240720326465</v>
       </c>
       <c r="D62" t="n">
-        <v>0.3743913316864461</v>
+        <v>0.7083865263369217</v>
       </c>
       <c r="E62" t="n">
-        <v>15</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>cbFICO</t>
+          <t>cbMosDlq</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>707.0~762.0</t>
+          <t>-0.0~4.0</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>1.260668147929439</v>
+        <v>-0.3884867715265001</v>
       </c>
       <c r="D63" t="n">
-        <v>0.3743913316864461</v>
+        <v>0.7083865263369217</v>
       </c>
       <c r="E63" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>cbFICO</t>
+          <t>cbMosDlq</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>762.0~inf</t>
+          <t>-inf~-0.001</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>1.763588592172946</v>
+        <v>0.1579747762509211</v>
       </c>
       <c r="D64" t="n">
-        <v>0.3743913316864461</v>
+        <v>0.7083865263369217</v>
       </c>
       <c r="E64" t="n">
-        <v>29</v>
+        <v>13</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>cbInq5Mos</t>
+          <t>cbMosDlq</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>-0.001~-0.0</t>
+          <t>39.0~inf</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>0.7664784535897855</v>
+        <v>0.3697470254738602</v>
       </c>
       <c r="D65" t="n">
-        <v>1.163711028782035</v>
+        <v>0.7083865263369217</v>
       </c>
       <c r="E65" t="n">
-        <v>36</v>
+        <v>17</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>cbInq5Mos</t>
+          <t>cbMosDlq</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>-0.0~1.0</t>
+          <t>4.0~39.0</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>0.5869571334945991</v>
+        <v>-0.03846628082411036</v>
       </c>
       <c r="D66" t="n">
-        <v>1.163711028782035</v>
+        <v>0.7083865263369217</v>
       </c>
       <c r="E66" t="n">
-        <v>30</v>
+        <v>9</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>cbInq5Mos</t>
+          <t>cbMosInq</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>-inf~-0.001</t>
+          <t>-0.001~-0.0</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>0.154150679796306</v>
+        <v>-0.0548632556085784</v>
       </c>
       <c r="D67" t="n">
-        <v>1.163711028782035</v>
+        <v>0.003408601656478899</v>
       </c>
       <c r="E67" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>cbInq5Mos</t>
+          <t>cbMosInq</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>1.0~2.0</t>
+          <t>-0.0~7.0</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>0.2557712601476568</v>
+        <v>0.1656197071601389</v>
       </c>
       <c r="D68" t="n">
-        <v>1.163711028782035</v>
+        <v>0.003408601656478899</v>
       </c>
       <c r="E68" t="n">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>cbInq5Mos</t>
+          <t>cbMosInq</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>13.0~inf</t>
+          <t>-inf~-0.001</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>-0.6061358034882809</v>
+        <v>0.5596157878904822</v>
       </c>
       <c r="D69" t="n">
-        <v>1.163711028782035</v>
+        <v>0.003408601656478899</v>
       </c>
       <c r="E69" t="n">
-        <v>-10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>cbInq5Mos</t>
+          <t>cbMosInq</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>2.0~3.0</t>
+          <t>7.0~inf</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>0.1103480571578621</v>
+        <v>1.481604540826943</v>
       </c>
       <c r="D70" t="n">
-        <v>1.163711028782035</v>
+        <v>0.003408601656478899</v>
       </c>
       <c r="E70" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>cbInq5Mos</t>
+          <t>cbPctGood</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>3.0~4.0</t>
+          <t>-0.001~86.0</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>-0.06062462181063718</v>
+        <v>-0.2556971964069784</v>
       </c>
       <c r="D71" t="n">
-        <v>1.163711028782035</v>
+        <v>0.2033154727587507</v>
       </c>
       <c r="E71" t="n">
         <v>8</v>
@@ -1933,250 +1933,250 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>cbInq5Mos</t>
+          <t>cbPctGood</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>4.0~13.0</t>
+          <t>-inf~-0.001</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>-0.358695373362934</v>
+        <v>-0.4168938038811993</v>
       </c>
       <c r="D72" t="n">
-        <v>1.163711028782035</v>
+        <v>0.2033154727587507</v>
       </c>
       <c r="E72" t="n">
-        <v>-2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>cbMosAvg</t>
+          <t>cbPctGood</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>-0.001~-0.0</t>
+          <t>86.0~91.0</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>0.3629054936526839</v>
+        <v>0.05908891636339926</v>
       </c>
       <c r="D73" t="n">
-        <v>0.9649810779893558</v>
+        <v>0.2033154727587507</v>
       </c>
       <c r="E73" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>cbMosAvg</t>
+          <t>cbPctGood</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>-0.0~1.0</t>
+          <t>91.0~97.0</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>0.4367176515756936</v>
+        <v>0.7556675374866363</v>
       </c>
       <c r="D74" t="n">
-        <v>0.9649810779893558</v>
+        <v>0.2033154727587507</v>
       </c>
       <c r="E74" t="n">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>cbMosAvg</t>
+          <t>cbPctGood</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>-inf~-0.001</t>
+          <t>97.0~inf</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>-0.1400792515807443</v>
+        <v>0.2248005525015409</v>
       </c>
       <c r="D75" t="n">
-        <v>0.9649810779893558</v>
+        <v>0.2033154727587507</v>
       </c>
       <c r="E75" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>cbMosAvg</t>
+          <t>cbTimeFile</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>1.0~3.0</t>
+          <t>-0.001~39.0</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>0.3313571359255232</v>
+        <v>-0.5463822467004612</v>
       </c>
       <c r="D76" t="n">
-        <v>0.9649810779893558</v>
+        <v>0.1237040236879398</v>
       </c>
       <c r="E76" t="n">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>cbMosAvg</t>
+          <t>cbTimeFile</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>25.0~63.0</t>
+          <t>-inf~-0.001</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>-0.1216071320826191</v>
+        <v>-0.2876820724234475</v>
       </c>
       <c r="D77" t="n">
-        <v>0.9649810779893558</v>
+        <v>0.1237040236879398</v>
       </c>
       <c r="E77" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>cbMosAvg</t>
+          <t>cbTimeFile</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>3.0~6.0</t>
+          <t>186.1~inf</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>0.3209077200512991</v>
+        <v>0.941886279001182</v>
       </c>
       <c r="D78" t="n">
-        <v>0.9649810779893558</v>
+        <v>0.1237040236879398</v>
       </c>
       <c r="E78" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>cbMosAvg</t>
+          <t>cbTimeFile</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>6.0~25.0</t>
+          <t>39.0~94.0</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>-0.01330396562546398</v>
+        <v>-0.1035131727755819</v>
       </c>
       <c r="D79" t="n">
-        <v>0.9649810779893558</v>
+        <v>0.1237040236879398</v>
       </c>
       <c r="E79" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>cbMosAvg</t>
+          <t>cbTimeFile</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>63.0~inf</t>
+          <t>94.0~186.1</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>-0.4700036291882356</v>
+        <v>0.2976821557603668</v>
       </c>
       <c r="D80" t="n">
-        <v>0.9649810779893558</v>
+        <v>0.1237040236879398</v>
       </c>
       <c r="E80" t="n">
-        <v>-3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>cbMosDlq</t>
+          <t>cbTimeFileYears</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>-0.001~-0.0</t>
+          <t>-0.001~2.0</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>-0.4855078157230469</v>
+        <v>-0.55043476178783</v>
       </c>
       <c r="D81" t="n">
-        <v>1.085928990574959</v>
+        <v>0.2296131172431497</v>
       </c>
       <c r="E81" t="n">
-        <v>-5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>cbMosDlq</t>
+          <t>cbTimeFileYears</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>-0.0~9.0</t>
+          <t>-inf~-0.001</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>-0.2837681730980282</v>
+        <v>-0.2876820724234475</v>
       </c>
       <c r="D82" t="n">
-        <v>1.085928990574959</v>
+        <v>0.2296131172431497</v>
       </c>
       <c r="E82" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>cbMosDlq</t>
+          <t>cbTimeFileYears</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>-inf~-0.001</t>
+          <t>14.0~inf</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>0.1580392135521808</v>
+        <v>0.913006656612277</v>
       </c>
       <c r="D83" t="n">
-        <v>1.085928990574959</v>
+        <v>0.2296131172431497</v>
       </c>
       <c r="E83" t="n">
         <v>15</v>
@@ -2185,40 +2185,40 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>cbMosDlq</t>
+          <t>cbTimeFileYears</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>64.0~inf</t>
+          <t>2.0~7.0</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>0.5930637219534641</v>
+        <v>-0.1169105113762201</v>
       </c>
       <c r="D84" t="n">
-        <v>1.085928990574959</v>
+        <v>0.2296131172431497</v>
       </c>
       <c r="E84" t="n">
-        <v>29</v>
+        <v>9</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>cbMosDlq</t>
+          <t>cbTimeFileYears</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>9.0~64.0</t>
+          <t>7.0~14.0</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>0.02097979046676507</v>
+        <v>0.2763448386242077</v>
       </c>
       <c r="D85" t="n">
-        <v>1.085928990574959</v>
+        <v>0.2296131172431497</v>
       </c>
       <c r="E85" t="n">
         <v>11</v>
@@ -2227,7 +2227,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>cbMosInq</t>
+          <t>cbUtilizn</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2236,40 +2236,40 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>-0.06484113877586589</v>
+        <v>0.2055992416436292</v>
       </c>
       <c r="D86" t="n">
-        <v>0.272007327015363</v>
+        <v>0.5304709774470813</v>
       </c>
       <c r="E86" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>cbMosInq</t>
+          <t>cbUtilizn</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>-0.0~5.0</t>
+          <t>-0.0~14.0</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>0.2071432099482654</v>
+        <v>1.042417730258088</v>
       </c>
       <c r="D87" t="n">
-        <v>0.272007327015363</v>
+        <v>0.5304709774470813</v>
       </c>
       <c r="E87" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>cbMosInq</t>
+          <t>cbUtilizn</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2278,895 +2278,223 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>0.7062192620740172</v>
+        <v>-0.4460610883325266</v>
       </c>
       <c r="D88" t="n">
-        <v>0.272007327015363</v>
+        <v>0.5304709774470813</v>
       </c>
       <c r="E88" t="n">
-        <v>16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>cbMosInq</t>
+          <t>cbUtilizn</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>10.0~inf</t>
+          <t>14.0~96.0</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>1.386294360994891</v>
+        <v>0.1434031410902038</v>
       </c>
       <c r="D89" t="n">
-        <v>0.272007327015363</v>
+        <v>0.5304709774470813</v>
       </c>
       <c r="E89" t="n">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>cbMosInq</t>
+          <t>cbUtilizn</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>5.0~8.0</t>
+          <t>96.0~inf</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>0.2231435512858765</v>
+        <v>-0.5658077581078741</v>
       </c>
       <c r="D90" t="n">
-        <v>0.272007327015363</v>
+        <v>0.5304709774470813</v>
       </c>
       <c r="E90" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>cbMosInq</t>
+          <t>dealLoanToVal</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>8.0~10.0</t>
+          <t>-inf~50.1</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>24.81761039906851</v>
+        <v>1.40399393813671</v>
       </c>
       <c r="D91" t="n">
-        <v>0.272007327015363</v>
+        <v>0.3890718018887464</v>
       </c>
       <c r="E91" t="n">
-        <v>205</v>
+        <v>25</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>cbPctGood</t>
+          <t>dealLoanToVal</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>-0.001~-0.0</t>
+          <t>50.1~70.6</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>-0.3522205935486925</v>
+        <v>0.660510251197664</v>
       </c>
       <c r="D92" t="n">
-        <v>0.3087598169301596</v>
+        <v>0.3890718018887464</v>
       </c>
       <c r="E92" t="n">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>cbPctGood</t>
+          <t>dealLoanToVal</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>-0.0~11.0</t>
+          <t>70.6~77.4</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>-23.02585092994046</v>
+        <v>0.2728669866421063</v>
       </c>
       <c r="D93" t="n">
-        <v>0.3087598169301596</v>
+        <v>0.3890718018887464</v>
       </c>
       <c r="E93" t="n">
-        <v>-195</v>
+        <v>12</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>cbPctGood</t>
+          <t>dealLoanToVal</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>-inf~-0.001</t>
+          <t>77.4~inf</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>-0.3920420877293751</v>
+        <v>-0.1403387708375491</v>
       </c>
       <c r="D94" t="n">
-        <v>0.3087598169301596</v>
+        <v>0.3890718018887464</v>
       </c>
       <c r="E94" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>cbPctGood</t>
+          <t>dealPctDown</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>11.0~87.0</t>
+          <t>-inf~16.8</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>-0.2122260278137308</v>
+        <v>-0.1801697724465584</v>
       </c>
       <c r="D95" t="n">
-        <v>0.3087598169301596</v>
+        <v>0.4585641585285222</v>
       </c>
       <c r="E95" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>cbPctGood</t>
+          <t>dealPctDown</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>87.0~91.0</t>
+          <t>16.8~27.0</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>0.01092907053000446</v>
+        <v>0.0872283673257974</v>
       </c>
       <c r="D96" t="n">
-        <v>0.3087598169301596</v>
+        <v>0.4585641585285222</v>
       </c>
       <c r="E96" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>cbPctGood</t>
+          <t>dealPctDown</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>91.0~95.0</t>
+          <t>27.0~49.9</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>0.6299682788896337</v>
+        <v>0.6105149159332927</v>
       </c>
       <c r="D97" t="n">
-        <v>0.3087598169301596</v>
+        <v>0.4585641585285222</v>
       </c>
       <c r="E97" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>cbPctGood</t>
+          <t>dealPctDown</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>95.0~inf</t>
+          <t>49.9~inf</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>0.232805462204983</v>
+        <v>1.386294361037748</v>
       </c>
       <c r="D98" t="n">
-        <v>0.3087598169301596</v>
+        <v>0.4585641585285222</v>
       </c>
       <c r="E98" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="inlineStr">
-        <is>
-          <t>cbTimeFile</t>
-        </is>
-      </c>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>-0.001~-0.0</t>
-        </is>
-      </c>
-      <c r="C99" t="n">
-        <v>-0.2876820724246974</v>
-      </c>
-      <c r="D99" t="n">
-        <v>0.2922168149130499</v>
-      </c>
-      <c r="E99" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>cbTimeFile</t>
-        </is>
-      </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>-0.0~30.0</t>
-        </is>
-      </c>
-      <c r="C100" t="n">
-        <v>-0.5402395089009321</v>
-      </c>
-      <c r="D100" t="n">
-        <v>0.2922168149130499</v>
-      </c>
-      <c r="E100" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>cbTimeFile</t>
-        </is>
-      </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>-inf~-0.001</t>
-        </is>
-      </c>
-      <c r="C101" t="n">
-        <v>0.06899287147314187</v>
-      </c>
-      <c r="D101" t="n">
-        <v>0.2922168149130499</v>
-      </c>
-      <c r="E101" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="inlineStr">
-        <is>
-          <t>cbTimeFile</t>
-        </is>
-      </c>
-      <c r="B102" t="inlineStr">
-        <is>
-          <t>112.0~183.0</t>
-        </is>
-      </c>
-      <c r="C102" t="n">
-        <v>0.2897291560479427</v>
-      </c>
-      <c r="D102" t="n">
-        <v>0.2922168149130499</v>
-      </c>
-      <c r="E102" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="inlineStr">
-        <is>
-          <t>cbTimeFile</t>
-        </is>
-      </c>
-      <c r="B103" t="inlineStr">
-        <is>
-          <t>183.0~188.0</t>
-        </is>
-      </c>
-      <c r="C103" t="n">
-        <v>1.335001066638656</v>
-      </c>
-      <c r="D103" t="n">
-        <v>0.2922168149130499</v>
-      </c>
-      <c r="E103" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="inlineStr">
-        <is>
-          <t>cbTimeFile</t>
-        </is>
-      </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>188.0~317.0</t>
-        </is>
-      </c>
-      <c r="C104" t="n">
-        <v>0.9035517060359723</v>
-      </c>
-      <c r="D104" t="n">
-        <v>0.2922168149130499</v>
-      </c>
-      <c r="E104" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="inlineStr">
-        <is>
-          <t>cbTimeFile</t>
-        </is>
-      </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>30.0~112.0</t>
-        </is>
-      </c>
-      <c r="C105" t="n">
-        <v>-0.1096431774383675</v>
-      </c>
-      <c r="D105" t="n">
-        <v>0.2922168149130499</v>
-      </c>
-      <c r="E105" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="inlineStr">
-        <is>
-          <t>cbTimeFile</t>
-        </is>
-      </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>317.0~inf</t>
-        </is>
-      </c>
-      <c r="C106" t="n">
-        <v>0.6632942173558971</v>
-      </c>
-      <c r="D106" t="n">
-        <v>0.2922168149130499</v>
-      </c>
-      <c r="E106" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="inlineStr">
-        <is>
-          <t>cbTimeFileYears</t>
-        </is>
-      </c>
-      <c r="B107" t="inlineStr">
-        <is>
-          <t>-0.001~1.0</t>
-        </is>
-      </c>
-      <c r="C107" t="n">
-        <v>-0.5642734581339583</v>
-      </c>
-      <c r="D107" t="n">
-        <v>-0.004793649552531688</v>
-      </c>
-      <c r="E107" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="inlineStr">
-        <is>
-          <t>cbTimeFileYears</t>
-        </is>
-      </c>
-      <c r="B108" t="inlineStr">
-        <is>
-          <t>-inf~-0.001</t>
-        </is>
-      </c>
-      <c r="C108" t="n">
-        <v>0.06899287147314187</v>
-      </c>
-      <c r="D108" t="n">
-        <v>-0.004793649552531688</v>
-      </c>
-      <c r="E108" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="inlineStr">
-        <is>
-          <t>cbTimeFileYears</t>
-        </is>
-      </c>
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>1.0~7.0</t>
-        </is>
-      </c>
-      <c r="C109" t="n">
-        <v>-0.1977064756117008</v>
-      </c>
-      <c r="D109" t="n">
-        <v>-0.004793649552531688</v>
-      </c>
-      <c r="E109" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="inlineStr">
-        <is>
-          <t>cbTimeFileYears</t>
-        </is>
-      </c>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>15.0~29.0</t>
-        </is>
-      </c>
-      <c r="C110" t="n">
-        <v>0.8960880244962018</v>
-      </c>
-      <c r="D110" t="n">
-        <v>-0.004793649552531688</v>
-      </c>
-      <c r="E110" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="inlineStr">
-        <is>
-          <t>cbTimeFileYears</t>
-        </is>
-      </c>
-      <c r="B111" t="inlineStr">
-        <is>
-          <t>29.0~inf</t>
-        </is>
-      </c>
-      <c r="C111" t="n">
-        <v>0.9985288300336835</v>
-      </c>
-      <c r="D111" t="n">
-        <v>-0.004793649552531688</v>
-      </c>
-      <c r="E111" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="inlineStr">
-        <is>
-          <t>cbTimeFileYears</t>
-        </is>
-      </c>
-      <c r="B112" t="inlineStr">
-        <is>
-          <t>7.0~9.0</t>
-        </is>
-      </c>
-      <c r="C112" t="n">
-        <v>0.1999252611932621</v>
-      </c>
-      <c r="D112" t="n">
-        <v>-0.004793649552531688</v>
-      </c>
-      <c r="E112" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="inlineStr">
-        <is>
-          <t>cbTimeFileYears</t>
-        </is>
-      </c>
-      <c r="B113" t="inlineStr">
-        <is>
-          <t>9.0~15.0</t>
-        </is>
-      </c>
-      <c r="C113" t="n">
-        <v>0.3749749413186573</v>
-      </c>
-      <c r="D113" t="n">
-        <v>-0.004793649552531688</v>
-      </c>
-      <c r="E113" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="inlineStr">
-        <is>
-          <t>cbUtilizn</t>
-        </is>
-      </c>
-      <c r="B114" t="inlineStr">
-        <is>
-          <t>-0.001~-0.0</t>
-        </is>
-      </c>
-      <c r="C114" t="n">
-        <v>0.1488456275825007</v>
-      </c>
-      <c r="D114" t="n">
-        <v>0.8050005725550949</v>
-      </c>
-      <c r="E114" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" t="inlineStr">
-        <is>
-          <t>cbUtilizn</t>
-        </is>
-      </c>
-      <c r="B115" t="inlineStr">
-        <is>
-          <t>-0.0~3.0</t>
-        </is>
-      </c>
-      <c r="C115" t="n">
-        <v>1.386294361034891</v>
-      </c>
-      <c r="D115" t="n">
-        <v>0.8050005725550949</v>
-      </c>
-      <c r="E115" t="n">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" t="inlineStr">
-        <is>
-          <t>cbUtilizn</t>
-        </is>
-      </c>
-      <c r="B116" t="inlineStr">
-        <is>
-          <t>-inf~-0.001</t>
-        </is>
-      </c>
-      <c r="C116" t="n">
-        <v>-0.4449439190261266</v>
-      </c>
-      <c r="D116" t="n">
-        <v>0.8050005725550949</v>
-      </c>
-      <c r="E116" t="n">
-        <v>-0</v>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" t="inlineStr">
-        <is>
-          <t>cbUtilizn</t>
-        </is>
-      </c>
-      <c r="B117" t="inlineStr">
-        <is>
-          <t>10.0~17.0</t>
-        </is>
-      </c>
-      <c r="C117" t="n">
-        <v>0.6632942173588381</v>
-      </c>
-      <c r="D117" t="n">
-        <v>0.8050005725550949</v>
-      </c>
-      <c r="E117" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" t="inlineStr">
-        <is>
-          <t>cbUtilizn</t>
-        </is>
-      </c>
-      <c r="B118" t="inlineStr">
-        <is>
-          <t>17.0~45.0</t>
-        </is>
-      </c>
-      <c r="C118" t="n">
-        <v>0.3724473390478827</v>
-      </c>
-      <c r="D118" t="n">
-        <v>0.8050005725550949</v>
-      </c>
-      <c r="E118" t="n">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" t="inlineStr">
-        <is>
-          <t>cbUtilizn</t>
-        </is>
-      </c>
-      <c r="B119" t="inlineStr">
-        <is>
-          <t>3.0~10.0</t>
-        </is>
-      </c>
-      <c r="C119" t="n">
-        <v>0.958254930907972</v>
-      </c>
-      <c r="D119" t="n">
-        <v>0.8050005725550949</v>
-      </c>
-      <c r="E119" t="n">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" t="inlineStr">
-        <is>
-          <t>cbUtilizn</t>
-        </is>
-      </c>
-      <c r="B120" t="inlineStr">
-        <is>
-          <t>45.0~69.0</t>
-        </is>
-      </c>
-      <c r="C120" t="n">
-        <v>0.05959209719602192</v>
-      </c>
-      <c r="D120" t="n">
-        <v>0.8050005725550949</v>
-      </c>
-      <c r="E120" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" t="inlineStr">
-        <is>
-          <t>cbUtilizn</t>
-        </is>
-      </c>
-      <c r="B121" t="inlineStr">
-        <is>
-          <t>69.0~98.0</t>
-        </is>
-      </c>
-      <c r="C121" t="n">
-        <v>-0.04292504471292807</v>
-      </c>
-      <c r="D121" t="n">
-        <v>0.8050005725550949</v>
-      </c>
-      <c r="E121" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" t="inlineStr">
-        <is>
-          <t>cbUtilizn</t>
-        </is>
-      </c>
-      <c r="B122" t="inlineStr">
-        <is>
-          <t>98.0~inf</t>
-        </is>
-      </c>
-      <c r="C122" t="n">
-        <v>-0.4978384281756437</v>
-      </c>
-      <c r="D122" t="n">
-        <v>0.8050005725550949</v>
-      </c>
-      <c r="E122" t="n">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" t="inlineStr">
-        <is>
-          <t>dealLoanToVal</t>
-        </is>
-      </c>
-      <c r="B123" t="inlineStr">
-        <is>
-          <t>-inf~42.1</t>
-        </is>
-      </c>
-      <c r="C123" t="n">
-        <v>1.435084525193132</v>
-      </c>
-      <c r="D123" t="n">
-        <v>0.9316905313373122</v>
-      </c>
-      <c r="E123" t="n">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" t="inlineStr">
-        <is>
-          <t>dealLoanToVal</t>
-        </is>
-      </c>
-      <c r="B124" t="inlineStr">
-        <is>
-          <t>42.1~48.6</t>
-        </is>
-      </c>
-      <c r="C124" t="n">
-        <v>2.4423470352279</v>
-      </c>
-      <c r="D124" t="n">
-        <v>0.9316905313373122</v>
-      </c>
-      <c r="E124" t="n">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" t="inlineStr">
-        <is>
-          <t>dealLoanToVal</t>
-        </is>
-      </c>
-      <c r="B125" t="inlineStr">
-        <is>
-          <t>48.6~53.1</t>
-        </is>
-      </c>
-      <c r="C125" t="n">
-        <v>1.152679509853298</v>
-      </c>
-      <c r="D125" t="n">
-        <v>0.9316905313373122</v>
-      </c>
-      <c r="E125" t="n">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" t="inlineStr">
-        <is>
-          <t>dealLoanToVal</t>
-        </is>
-      </c>
-      <c r="B126" t="inlineStr">
-        <is>
-          <t>53.1~71.0</t>
-        </is>
-      </c>
-      <c r="C126" t="n">
-        <v>0.5496654570389787</v>
-      </c>
-      <c r="D126" t="n">
-        <v>0.9316905313373122</v>
-      </c>
-      <c r="E126" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" t="inlineStr">
-        <is>
-          <t>dealLoanToVal</t>
-        </is>
-      </c>
-      <c r="B127" t="inlineStr">
-        <is>
-          <t>71.0~75.6</t>
-        </is>
-      </c>
-      <c r="C127" t="n">
-        <v>0.2231435512929597</v>
-      </c>
-      <c r="D127" t="n">
-        <v>0.9316905313373122</v>
-      </c>
-      <c r="E127" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" t="inlineStr">
-        <is>
-          <t>dealLoanToVal</t>
-        </is>
-      </c>
-      <c r="B128" t="inlineStr">
-        <is>
-          <t>75.6~83.8</t>
-        </is>
-      </c>
-      <c r="C128" t="n">
-        <v>0.03509131980749718</v>
-      </c>
-      <c r="D128" t="n">
-        <v>0.9316905313373122</v>
-      </c>
-      <c r="E128" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129" t="inlineStr">
-        <is>
-          <t>dealLoanToVal</t>
-        </is>
-      </c>
-      <c r="B129" t="inlineStr">
-        <is>
-          <t>83.8~89.5</t>
-        </is>
-      </c>
-      <c r="C129" t="n">
-        <v>-0.1571855835056183</v>
-      </c>
-      <c r="D129" t="n">
-        <v>0.9316905313373122</v>
-      </c>
-      <c r="E129" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" t="inlineStr">
-        <is>
-          <t>dealLoanToVal</t>
-        </is>
-      </c>
-      <c r="B130" t="inlineStr">
-        <is>
-          <t>89.5~inf</t>
-        </is>
-      </c>
-      <c r="C130" t="n">
-        <v>-0.1780297046931067</v>
-      </c>
-      <c r="D130" t="n">
-        <v>0.9316905313373122</v>
-      </c>
-      <c r="E130" t="n">
-        <v>5</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>